<commit_message>
Included Customer creation script
</commit_message>
<xml_diff>
--- a/extFiles/Design_eureQa.xlsx
+++ b/extFiles/Design_eureQa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\riverSand-SKUCreation\extFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50610FBF-E7F0-4AD5-887A-76415721D960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F56938-4DC1-4EFC-A241-FE76D9115DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" tabRatio="796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refineSearch" sheetId="2" r:id="rId1"/>
@@ -19,15 +19,14 @@
     <sheet name="EntityDownload" sheetId="5" r:id="rId4"/>
     <sheet name="OpenEntityManage" sheetId="6" r:id="rId5"/>
     <sheet name="Misc" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
-    <sheet name="Design_eureQa" sheetId="1" r:id="rId8"/>
+    <sheet name="Design_eureQa" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="106">
   <si>
     <t>refineSearch.xlsx</t>
   </si>
@@ -345,22 +344,13 @@
   </si>
   <si>
     <t>TCo1</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>adb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,14 +485,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -807,7 +789,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -850,14 +832,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -891,7 +871,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1214,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F0EA7A-366F-4408-9968-77961CB368AA}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1765,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,234 +1958,204 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F85E24A-5A57-42EC-A33C-8D154BBF32A0}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="39.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>108</v>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>88</v>
       </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="adb@" xr:uid="{EF65FCD7-FFD7-4C79-B6C8-AC04A3414479}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94CE1FA-B891-4B78-BC8A-63C66DBFEC07}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>

</xml_diff>